<commit_message>
Presque la fin des commandes BSPD
</commit_message>
<xml_diff>
--- a/EL - Electrical/Autre/BSPD/Version FSG/BOM_BSPD.xlsx
+++ b/EL - Electrical/Autre/BSPD/Version FSG/BOM_BSPD.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\STUF2019\EL - Electrical\Autre\BSPD\Version FSG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D94C61-44CF-4E1F-B735-FF08CB7218D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754A0305-CB3B-455D-A695-9BBF718FF66A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FSG_2019_BSPD_0.2_SMD" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
   <si>
     <t>Qty</t>
   </si>
@@ -61,9 +61,6 @@
     <t>100k</t>
   </si>
   <si>
-    <t>100n</t>
-  </si>
-  <si>
     <t>C-EUC0603</t>
   </si>
   <si>
@@ -76,21 +73,12 @@
     <t>10k</t>
   </si>
   <si>
-    <t>10Âµ</t>
-  </si>
-  <si>
-    <t>C-EUC1206</t>
-  </si>
-  <si>
     <t>C1206</t>
   </si>
   <si>
     <t>C-EUC1206K</t>
   </si>
   <si>
-    <t>C1206K</t>
-  </si>
-  <si>
     <t>20k</t>
   </si>
   <si>
@@ -215,6 +203,36 @@
   </si>
   <si>
     <t>153-1886</t>
+  </si>
+  <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>10µF</t>
+  </si>
+  <si>
+    <t>173-2966</t>
+  </si>
+  <si>
+    <t>740-8802</t>
+  </si>
+  <si>
+    <t>740-8798</t>
+  </si>
+  <si>
+    <t>679-0532</t>
+  </si>
+  <si>
+    <t>679-0285</t>
+  </si>
+  <si>
+    <t>678-9667</t>
+  </si>
+  <si>
+    <t>136-7681</t>
+  </si>
+  <si>
+    <t>172-6888</t>
   </si>
 </sst>
 </file>
@@ -571,7 +589,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -729,6 +747,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -815,11 +842,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -866,7 +893,35 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1205,10 +1260,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,16 +1292,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>56</v>
-      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -1261,11 +1316,13 @@
         <v>7</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="14"/>
+        <v>53</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>63</v>
+      </c>
       <c r="K2" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1285,11 +1342,13 @@
         <v>11</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" s="13"/>
+        <v>53</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>65</v>
+      </c>
       <c r="K3" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1309,37 +1368,41 @@
         <v>11</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" s="13"/>
+        <v>53</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" s="13"/>
+        <v>53</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>9</v>
@@ -1351,207 +1414,217 @@
         <v>11</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" s="13"/>
+        <v>53</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G7" s="13"/>
+        <v>53</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>4</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="7" t="s">
+      <c r="E10" s="6"/>
+      <c r="F10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>2</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>3</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>2</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>1</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="13"/>
+      <c r="C12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>2</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="6" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>3</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>62</v>
-      </c>
+      <c r="C13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="13"/>
     </row>
-    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
         <v>1</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="8" t="s">
+      <c r="D14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>3</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="13"/>
+      <c r="G14" s="13" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>39</v>
-      </c>
       <c r="F15" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>60</v>
+        <v>53</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>40</v>
@@ -1559,14 +1632,12 @@
       <c r="D16" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>42</v>
-      </c>
+      <c r="E16" s="6"/>
       <c r="F16" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1574,23 +1645,25 @@
         <v>1</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="6"/>
       <c r="F17" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>63</v>
+        <v>53</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>1</v>
       </c>
@@ -1601,58 +1674,51 @@
         <v>47</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>49</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E18" s="6"/>
       <c r="F18" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
-        <v>1</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>64</v>
+        <v>53</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F2:F19">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="oui">
+  <conditionalFormatting sqref="F2:F4 F6:F18">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="oui">
       <formula>NOT(ISERROR(SEARCH("oui",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F19">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Je sais pas">
+  <conditionalFormatting sqref="F2:F4 F6:F18">
+    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="Je sais pas">
       <formula>NOT(ISERROR(SEARCH("Je sais pas",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="non">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="non">
       <formula>NOT(ISERROR(SEARCH("non",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="oui">
+    <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="oui">
       <formula>NOT(ISERROR(SEARCH("oui",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="oui">
+      <formula>NOT(ISERROR(SEARCH("oui",F5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Je sais pas">
+      <formula>NOT(ISERROR(SEARCH("Je sais pas",F5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="non">
+      <formula>NOT(ISERROR(SEARCH("non",F5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="oui">
+      <formula>NOT(ISERROR(SEARCH("oui",F5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F19" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F18" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$K$1:$K$3</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fin des commandes RS ?
</commit_message>
<xml_diff>
--- a/EL - Electrical/Autre/BSPD/Version FSG/BOM_BSPD.xlsx
+++ b/EL - Electrical/Autre/BSPD/Version FSG/BOM_BSPD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\STUF2019\EL - Electrical\Autre\BSPD\Version FSG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754A0305-CB3B-455D-A695-9BBF718FF66A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F0C6B5-22A9-466E-A80F-4156F7E534CB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="72">
   <si>
     <t>Qty</t>
   </si>
@@ -233,13 +233,16 @@
   </si>
   <si>
     <t>172-6888</t>
+  </si>
+  <si>
+    <t>Pas exactement le même modèle mais ok</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -389,6 +392,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -589,7 +598,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -748,12 +757,40 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFFFFFFF"/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -801,7 +838,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -814,9 +851,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -845,8 +879,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1263,7 +1306,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,52 +1316,55 @@
     <col min="5" max="5" width="27.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" customWidth="1"/>
+    <col min="9" max="9" width="1.7109375" customWidth="1"/>
+    <col min="10" max="10" width="2.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>48</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="16" t="s">
         <v>63</v>
       </c>
       <c r="K2" s="3" t="s">
@@ -1326,25 +1372,25 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>65</v>
       </c>
       <c r="K3" s="4" t="s">
@@ -1352,335 +1398,340 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>5</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="12" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>11</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="12" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>2</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="12" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>4</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="12" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>2</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7" t="s">
+      <c r="E10" s="5"/>
+      <c r="F10" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="12" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>2</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7" t="s">
+      <c r="E11" s="5"/>
+      <c r="F11" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="12" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>1</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="7" t="s">
+      <c r="E13" s="5"/>
+      <c r="F13" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="13"/>
+      <c r="G13" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>1</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="12" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>3</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="17" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+      <c r="A16" s="5">
         <v>1</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="7" t="s">
+      <c r="E16" s="5"/>
+      <c r="F16" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="13" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="A17" s="5">
         <v>1</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+      <c r="A18" s="5">
         <v>1</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="7" t="s">
+      <c r="E18" s="5"/>
+      <c r="F18" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="12" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>